<commit_message>
Updated test data sheet for TC151,60 and NGC-543
</commit_message>
<xml_diff>
--- a/Test Data/TC_151_Verify_Battery_Standby_And_Alarm_Load_On_Addition_Deletion_Of_Devices_In_Zetfast.xlsx
+++ b/Test Data/TC_151_Verify_Battery_Standby_And_Alarm_Load_On_Addition_Deletion_Of_Devices_In_Zetfast.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jbhasip\Desktop\NGConsys Automation_01_02_2019\Test Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\consys-uiauto\Test Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{900A5E4A-28D1-4E9C-A1B9-D4EDA9034AF0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13800" windowHeight="5604"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Add Panels" sheetId="6" r:id="rId1"/>
@@ -131,7 +132,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -547,11 +548,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+      <selection activeCell="H4" sqref="H4:L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -620,6 +621,13 @@
       <c r="E4" s="14"/>
       <c r="F4" s="14"/>
       <c r="G4" s="14"/>
+      <c r="H4" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="I4" s="15"/>
+      <c r="J4" s="15"/>
+      <c r="K4" s="15"/>
+      <c r="L4" s="15"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C5" s="3"/>
@@ -629,30 +637,38 @@
       <c r="E5" s="14"/>
       <c r="F5" s="14"/>
       <c r="G5" s="14"/>
-      <c r="H5" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="I5" s="15"/>
-      <c r="J5" s="15"/>
-      <c r="K5" s="15"/>
-      <c r="L5" s="15"/>
+      <c r="H5" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="I5" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="J5" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="K5" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="L5" s="11" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="2"/>
-      <c r="H6" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="I6" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="J6" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="K6" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="L6" s="11" t="s">
-        <v>32</v>
+      <c r="H6" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="J6" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="K6" s="10">
+        <v>0.09</v>
+      </c>
+      <c r="L6" s="10">
+        <v>0.09</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
@@ -678,19 +694,19 @@
         <v>15</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="I7" s="6" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="J7" s="6" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="K7" s="10">
-        <v>0.09</v>
+        <v>0.2</v>
       </c>
       <c r="L7" s="10">
-        <v>0.09</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
@@ -716,35 +732,18 @@
         <v>0.38700000000000001</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="I8" s="6" t="s">
         <v>23</v>
       </c>
       <c r="J8" s="6" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="K8" s="10">
         <v>0.2</v>
       </c>
       <c r="L8" s="10">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="H9" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="I9" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="J9" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="K9" s="10">
-        <v>0.2</v>
-      </c>
-      <c r="L9" s="10">
         <v>0.2</v>
       </c>
     </row>

</xml_diff>